<commit_message>
release 0.1.2 4.9b added w Zohaib Mughal
</commit_message>
<xml_diff>
--- a/Output 2/Indicator_Map_With_Signals_CLEAN.xlsx
+++ b/Output 2/Indicator_Map_With_Signals_CLEAN.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,17 +454,47 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>PriceVol_Reason</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>MACD_Signal</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>MACD_Reason</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Bollinger_Signal</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Bollinger_Reason</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Volume_Signal</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Volume_Reason</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Overall_Signal</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Signal_Reasoning</t>
         </is>
       </c>
     </row>
@@ -484,17 +514,47 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>Trend: uptrend, Volatility: 15.02854220982136</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Sell</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Trend: Neutral, Histogram Strength: -1.95</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Band: neutral, Volatility: 15.02854220982136</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Trend: downtrend</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>PriceVol: buy (+0.40) | MACD: sell (-0.25) | Bollinger: sell (-0.20) | Volume: sell (-0.15)</t>
         </is>
       </c>
     </row>
@@ -514,17 +574,47 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>Trend: downtrend, Volatility: 15.47683199402998</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Sell</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Trend: Neutral, Histogram Strength: -3.97</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Band: neutral, Volatility: 15.47683199402998</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Trend: downtrend</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>PriceVol: sell (-0.40) | MACD: sell (-0.25) | Bollinger: sell (-0.20) | Volume: sell (-0.15)</t>
         </is>
       </c>
     </row>
@@ -544,17 +634,47 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>Trend: downtrend, Volatility: 25.65931112908225</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Buy</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Trend: Neutral, Histogram Strength: -8.8</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Band: oversold, Volatility: 25.65931112908225</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Trend: downtrend</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>PriceVol: sell (-0.40) | MACD: sell (-0.25) | Bollinger: buy (+0.20) | Volume: sell (-0.15)</t>
         </is>
       </c>
     </row>
@@ -574,17 +694,47 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>Trend: uptrend, Volatility: 11.13681988463755</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Sell</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Trend: Sell, Histogram Strength: -4.05</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Band: neutral, Volatility: 11.13681988463755</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Trend: uptrend</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>PriceVol: buy (+0.40) | MACD: sell (-0.25) | Bollinger: sell (-0.20) | Volume: buy (+0.15)</t>
         </is>
       </c>
     </row>
@@ -604,17 +754,47 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>Trend: downtrend, Volatility: 11.88190320653737</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Sell</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Trend: Sell, Histogram Strength: 1.83</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Band: neutral, Volatility: 11.88190320653737</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Trend: uptrend</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>PriceVol: sell (-0.40) | MACD: sell (-0.25) | Bollinger: sell (-0.20) | Volume: buy (+0.15)</t>
         </is>
       </c>
     </row>
@@ -629,7 +809,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -655,17 +835,47 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>PriceVol_Reason</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>MACD_Signal</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>MACD_Reason</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Bollinger_Signal</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Bollinger_Reason</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Volume_Signal</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Volume_Reason</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Overall_Signal</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Signal_Reasoning</t>
         </is>
       </c>
     </row>
@@ -685,17 +895,47 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>Trend: uptrend, Volatility: 0.840093532207674</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>buy</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Buy</t>
-        </is>
-      </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Trend: Buy, Histogram Strength: 0.39</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Band: neutral, Volatility: 0.840093532207674</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Trend: downtrend</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>PriceVol: buy (+0.40) | MACD: buy (+0.25) | Bollinger: buy (+0.20) | Volume: sell (-0.15)</t>
         </is>
       </c>
     </row>
@@ -715,17 +955,47 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
+          <t>Trend: downtrend, Volatility: 0.9731857357105586</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>buy</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Buy</t>
-        </is>
-      </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Trend: Buy, Histogram Strength: 0.21</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Band: neutral, Volatility: 0.9731857357105586</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Trend: uptrend</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>PriceVol: sell (-0.40) | MACD: buy (+0.25) | Bollinger: buy (+0.20) | Volume: buy (+0.15)</t>
         </is>
       </c>
     </row>
@@ -745,17 +1015,47 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>Trend: uptrend, Volatility: 2.476546174086182</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Sell</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Buy</t>
+          <t>Trend: Neutral, Histogram Strength: 0.19</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Band: overbought, Volatility: 2.476546174086182</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Trend: uptrend</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>PriceVol: buy (+0.40) | MACD: sell (-0.25) | Bollinger: sell (-0.20) | Volume: buy (+0.15)</t>
         </is>
       </c>
     </row>
@@ -775,17 +1075,47 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
+          <t>Trend: uptrend, Volatility: 2.935980407356449</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
           <t>buy</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
-      </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Trend: Buy, Histogram Strength: 0.93</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Band: overbought, Volatility: 2.935980407356449</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Trend: uptrend</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>PriceVol: buy (+0.40) | MACD: buy (+0.25) | Bollinger: sell (-0.20) | Volume: buy (+0.15)</t>
         </is>
       </c>
     </row>
@@ -805,17 +1135,47 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
+          <t>Trend: uptrend, Volatility: 1.772159027584043</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
           <t>buy</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Buy</t>
-        </is>
-      </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Trend: Buy, Histogram Strength: 0.34</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Band: neutral, Volatility: 1.772159027584043</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Trend: downtrend</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>PriceVol: buy (+0.40) | MACD: buy (+0.25) | Bollinger: buy (+0.20) | Volume: sell (-0.15)</t>
         </is>
       </c>
     </row>
@@ -830,7 +1190,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -856,17 +1216,47 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>PriceVol_Reason</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>MACD_Signal</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>MACD_Reason</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Bollinger_Signal</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Bollinger_Reason</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Volume_Signal</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Volume_Reason</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Overall_Signal</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Signal_Reasoning</t>
         </is>
       </c>
     </row>
@@ -886,17 +1276,47 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>Trend: downtrend, Volatility: 26.23960165928774</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Sell</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Trend: Neutral, Histogram Strength: -7.68</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Band: neutral, Volatility: 26.23960165928774</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Trend: uptrend</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>PriceVol: sell (-0.40) | MACD: sell (-0.25) | Bollinger: sell (-0.20) | Volume: buy (+0.15)</t>
         </is>
       </c>
     </row>
@@ -916,17 +1336,47 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>Trend: uptrend, Volatility: 11.07897708876292</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Sell</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Trend: Neutral, Histogram Strength: -2.91</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Band: neutral, Volatility: 11.07897708876292</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Trend: uptrend</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>PriceVol: buy (+0.40) | MACD: sell (-0.25) | Bollinger: sell (-0.20) | Volume: buy (+0.15)</t>
         </is>
       </c>
     </row>
@@ -946,17 +1396,47 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>Trend: downtrend, Volatility: 17.71938661197847</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Sell</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Trend: Neutral, Histogram Strength: -6.47</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Band: neutral, Volatility: 17.71938661197847</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Trend: uptrend</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>PriceVol: sell (-0.40) | MACD: sell (-0.25) | Bollinger: sell (-0.20) | Volume: buy (+0.15)</t>
         </is>
       </c>
     </row>
@@ -976,17 +1456,47 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>Trend: uptrend, Volatility: 14.21137321202383</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Sell</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Trend: Neutral, Histogram Strength: -6.27</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Band: neutral, Volatility: 14.21137321202383</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Trend: uptrend</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>PriceVol: buy (+0.40) | MACD: sell (-0.25) | Bollinger: sell (-0.20) | Volume: buy (+0.15)</t>
         </is>
       </c>
     </row>
@@ -1006,17 +1516,47 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>Trend: uptrend, Volatility: 25.30465155808687</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Sell</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Trend: Sell, Histogram Strength: 2.52</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Band: neutral, Volatility: 25.30465155808687</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Trend: uptrend</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>PriceVol: buy (+0.40) | MACD: sell (-0.25) | Bollinger: sell (-0.20) | Volume: buy (+0.15)</t>
         </is>
       </c>
     </row>
@@ -1031,7 +1571,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1057,17 +1597,47 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>PriceVol_Reason</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>MACD_Signal</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>MACD_Reason</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Bollinger_Signal</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Bollinger_Reason</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Volume_Signal</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Volume_Reason</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Overall_Signal</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Signal_Reasoning</t>
         </is>
       </c>
     </row>
@@ -1087,17 +1657,47 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>Trend: uptrend, Volatility: 0.920212190850825</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Buy</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Trend: Neutral, Histogram Strength: -0.31</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Band: neutral, Volatility: 0.920212190850825</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Trend: uptrend</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>PriceVol: buy (+0.40) | MACD: sell (-0.25) | Bollinger: buy (+0.20) | Volume: buy (+0.15)</t>
         </is>
       </c>
     </row>
@@ -1117,17 +1717,47 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>Trend: uptrend, Volatility: 1.526912539984496</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Buy</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Trend: Neutral, Histogram Strength: -0.41</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Band: neutral, Volatility: 1.526912539984496</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Trend: downtrend</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>PriceVol: buy (+0.40) | MACD: sell (-0.25) | Bollinger: buy (+0.20) | Volume: sell (-0.15)</t>
         </is>
       </c>
     </row>
@@ -1147,17 +1777,47 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>Trend: downtrend, Volatility: 0.7703122434318123</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Buy</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Trend: Neutral, Histogram Strength: -0.3</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Band: neutral, Volatility: 0.7703122434318123</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Trend: downtrend</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>PriceVol: sell (-0.40) | MACD: sell (-0.25) | Bollinger: buy (+0.20) | Volume: sell (-0.15)</t>
         </is>
       </c>
     </row>
@@ -1177,17 +1837,47 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>Trend: uptrend, Volatility: 0.6405838111032902</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Buy</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Trend: Neutral, Histogram Strength: -0.01</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Band: neutral, Volatility: 0.6405838111032902</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Trend: downtrend</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>PriceVol: buy (+0.40) | MACD: sell (-0.25) | Bollinger: buy (+0.20) | Volume: sell (-0.15)</t>
         </is>
       </c>
     </row>
@@ -1207,17 +1897,47 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>Trend: uptrend, Volatility: 0.9047546365622828</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Buy</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Trend: Sell, Histogram Strength: 0.04</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Band: neutral, Volatility: 0.9047546365622828</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Trend: downtrend</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>PriceVol: buy (+0.40) | MACD: sell (-0.25) | Bollinger: buy (+0.20) | Volume: sell (-0.15)</t>
         </is>
       </c>
     </row>

</xml_diff>